<commit_message>
Added perks to Excel Sheet, will add them to march later today
</commit_message>
<xml_diff>
--- a/perks.xlsx
+++ b/perks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fanfics\Tools\The March of Civilization Builder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fanfics\Tools\The March of Civilization Builder\March of Civilization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C86A546-7745-45EE-A94C-91A635272C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787F116E-0831-4FFF-ACE7-E0943BED1409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{03648907-44A0-47E6-BAD5-79650EC445A4}"/>
+    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{03648907-44A0-47E6-BAD5-79650EC445A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="17" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="791">
   <si>
     <t>Comeback Kid</t>
   </si>
@@ -2224,6 +2224,222 @@
   </si>
   <si>
     <t>You know how to create systems that can transmit packets of space at a faster-than-light speed and 'bounce back' after reaching a specific range. This allows signals and various events to operate at a range, allowing you to 'propagate' the effect of sensors at FTL speeds</t>
+  </si>
+  <si>
+    <t>Fission Works</t>
+  </si>
+  <si>
+    <t>You have the designs, knowledge and training to make all of Fission Work's wide gamut of fission-based nuclear reactors and radioisotope thermoelectric generators: ranging from muncipal solid-core designs to gas-core fission and ultra-light manportable nuclear power units.</t>
+  </si>
+  <si>
+    <t>You are inflicted with a dream, a dream of a love-letter to the Human form, arms and legs made mobile through designed artifice, then cladded in armor, and moved by mechanisms fueled by engineered power sources. Designs of leg, and arm drive trains come to you, as is the dizzingly complex systems or software required to let it keep it's balance, and most importantly: to move. This is the skill to make arms and legs that work like a human reflected into your chosen mechanical art, but other "exotic" forms are not too hard to puzzle out, so long as they got something like legs and arms.</t>
+  </si>
+  <si>
+    <t>Mechatronics In Motion</t>
+  </si>
+  <si>
+    <t>Soul of the Engine</t>
+  </si>
+  <si>
+    <t>You know how to design and make the gamut of techniques of garnering energy from combustion: engines, fuel cells, turbines and all. If it burns, you can think of a few ways to make it into motion.</t>
+  </si>
+  <si>
+    <t>There are a great many ways to provide municipal power to a town, a city, a country, or even a world. The Civil Engineering required to tap into Geothermal springs, or truckloads of coal, or a fusion reactor or any large-scale municipal power system into the electricity fed to the needs of the people come to you easily.</t>
+  </si>
+  <si>
+    <t>Power To The People</t>
+  </si>
+  <si>
+    <t>Accelerate the Projectile</t>
+  </si>
+  <si>
+    <t>Bolts, Arrows, Bullets, Flechettes and more are all under your perview. You have a grasp on engineering everything required to make a device capable of launching a projectile using explosive-combustion or muscle-power in its many forms. Using more exotic acceleration methods come to you more easily, as well.</t>
+  </si>
+  <si>
+    <t>Talk and See with Radios and Lasers</t>
+  </si>
+  <si>
+    <t>You have the knowledge of using Electromagnetic frequencies, most often Radio and Light waves, to communicate, and sense. This most often manifests in radio wave and laser communication, and RADAR/LADAR systems. Necessarily, this comes with the knowledge to protect and counter against such equipment, like using Electromagnetic Countermeasures or Electromagnetic Pulse Generating weapons.</t>
+  </si>
+  <si>
+    <t>Make Your Artifical Gravity</t>
+  </si>
+  <si>
+    <t>The applied engineering of scientific study of Gravitics made manifest: A series of designs towards supplying artifical gravity deck-plates, mass-tractor beams, kilometers wide inertial syncronization fields, and crude examples of gravitic weapons that show effective performance comparable to magnetic railgun weapons due to their imprecise manipulation of the gravitational fields that would otherwise be implemented into pinnacle weapons. You can make a devestating maul with this.</t>
+  </si>
+  <si>
+    <t>Song Series Weaponized Accoustics</t>
+  </si>
+  <si>
+    <t>The sonic weapons of a enlightened era, including examples of precise narrow-beam sonic pulse weapons capable of nonlethally disabling a targeted individual through lighter armor by temporarily shutting down their nervous system. Comes in a wide variety of packages most of them man portable, as well as more primitive examples that are only effective against targets that can hear with more traditional effects-- afflicting nausea and hearing loss.</t>
+  </si>
+  <si>
+    <t>Ink to Paper</t>
+  </si>
+  <si>
+    <t>The gamut of designs to put printed materials into the hands of the people are available to you, running from primitive printing presses on parchment to typewriters and ball-point pens to cutting edge paper-preparing chemical processes, and full color gloss printers. the many, varied steps of turning raw materials into the written word (or picture) are available to you.</t>
+  </si>
+  <si>
+    <t>The Coastguard Supply</t>
+  </si>
+  <si>
+    <t>A coastguard requires a great many vehicles, equipment and systems to run, ones that you do not have to make designs for now. You have been given all the tested and used designs on functional ships, boats, buildings, helicopters and the varied equipment that would enable the day to day operations of a coastguard or similar nautical rescue service.</t>
+  </si>
+  <si>
+    <t>Antimatter</t>
+  </si>
+  <si>
+    <t>Antimatter is volatile, and the ultimate storage mechanism for harnessable energy in hard-science environments. You know the science behind how to produce, store, and harness antimatter in all its various quantities. the smallest amounts are most economically usable for radiation medicine, but higher orders of magnetitude have obvious manufacturing, scientific, and miltiary applications.</t>
+  </si>
+  <si>
+    <t>Subtle signals</t>
+  </si>
+  <si>
+    <t>You can pick up what is being put down - to an extent beyond what is merely physically possible. This not only allows you to understand the subtle nuances of communication, but also absorb and assimilate the psionic component making you a better student.</t>
+  </si>
+  <si>
+    <t>Universal Simulation Module</t>
+  </si>
+  <si>
+    <t>You know how to create a extremely computationally intensive software package that can simulate the local universe with respect to the actions of the people inserted into it. Your understanding of this system allows you to identify various components, allowing you to extract internal functionality for any other purpose.</t>
+  </si>
+  <si>
+    <t>You are able to control your body incredibly preciesly first on the level of individual voluntary muscle groups, then to the level of nomally subconcious aspects such as metabolism, then to normally involuntary processes such as your heartbeat and hormones and finally on a cellular level.</t>
+  </si>
+  <si>
+    <t>Precision Body Control</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>You know how to describe problems in a rigorous manner. Though this may seem a simple thing, this allows you to break down complex procedures as a simple set of logical processes which are easily achieved through computation of all kinds.</t>
+  </si>
+  <si>
+    <t>Shapeshifting</t>
+  </si>
+  <si>
+    <t>You know how to create spells and enchantments that allow the target to take on another form, first simply others of their own kin, then any others of their own kind (animate remains animate and inanimate remains inanimate), then finally anything at all</t>
+  </si>
+  <si>
+    <t>Mystic Alchemy</t>
+  </si>
+  <si>
+    <t>You know how to take your akills into a realm that is often beyond the reach of most alchemists. To effect the world beyond the physical and reach for what lies beyond the material world. This allows you to apply alchemical principles to various supernatural forces, starting with Ki, then magic, then spiritual energy and finally the conceptual underpinnings of reality itself.</t>
+  </si>
+  <si>
+    <t>Spiritual Entities</t>
+  </si>
+  <si>
+    <t>You know how to create independent spiritual entities, self contained souls with enough power to act upon the physical world. These are fully independent entities with agency and the ability to act on your behalf or those who you assign them to, while still remaining undetectable to anyone without spiritual senses.</t>
+  </si>
+  <si>
+    <t>Spiritual Guardians</t>
+  </si>
+  <si>
+    <t>You know how to create autonomous subsections of a soul, granting it a protector and guardian that works constantly and independently of the soul itself. These guardians are not actually seperate from the soul and can grow alongside it.</t>
+  </si>
+  <si>
+    <t>Splicing</t>
+  </si>
+  <si>
+    <t>You have a deep understanding of how genetics translate into phenotypic expression. It takes you only a little experimentation to isolate what specific gentics are resposible for various biological structures and you have a knack for integrating those same structures into others - even into mature specimen.</t>
+  </si>
+  <si>
+    <t>Kaiju</t>
+  </si>
+  <si>
+    <t>There are creatures, monstrous creatures that defy any extant concept of biological limitation. You understand these creations, allowing you to creatures of immense size and strength.</t>
+  </si>
+  <si>
+    <t>Unending Endurance</t>
+  </si>
+  <si>
+    <t>Regardless of how long you have been working, and how much you have been exerting yourself, so long as you are in good health you can continue to work. This removes your need for food and sleep.</t>
+  </si>
+  <si>
+    <t>Hammerspace</t>
+  </si>
+  <si>
+    <t>You know how to creates pocket realms that are integrated into the natural functions of living beings, allowing them to store items in a convenient and weightless manner.</t>
+  </si>
+  <si>
+    <t>Impossible Proportions</t>
+  </si>
+  <si>
+    <t>You know how to alter the internal geometry of beings and objects in such a way that allows them to take on forms far larger than they seem to be able to at first.</t>
+  </si>
+  <si>
+    <t>Spooky Action</t>
+  </si>
+  <si>
+    <t>Mystic Places</t>
+  </si>
+  <si>
+    <t>You have a good sense of how to generate forces at a distance, from telekineisis to dealing damage directly, you can easily design spells and artefacts to achieve these feats.</t>
+  </si>
+  <si>
+    <t>Anchoring magical effects to places is no mean feat - indeed most such places are born of immense magical exposure over a great deal of time. Still, you know how to tie your workings into the ambient supplies of magic making them self-sustaining</t>
+  </si>
+  <si>
+    <t>Pulsar Series Laser Weapons</t>
+  </si>
+  <si>
+    <t>Accrection Series Plasma Weapons</t>
+  </si>
+  <si>
+    <t>Sol-Series Fusion Plants</t>
+  </si>
+  <si>
+    <t>Sunshine in a Can</t>
+  </si>
+  <si>
+    <t>Big Red Button</t>
+  </si>
+  <si>
+    <t>You have access to the plans and understanding necessary to make a wide variety of fission-based weaponry, capable of acting as tactical munitions to strategic options - on a planet and even beyond it. Indeed, this collection even includes systems that could be used for civilian purposes, though only if the timeline accounts for the fallout.</t>
+  </si>
+  <si>
+    <t>You know how to create a large variety of fusion explosives for uses that range from civilian to strategic. These can scale from man-portable anti-materiel grenades to black-navy straegic weapons capable of destroying orbital installations. In addition to the plans, you also have the knowledge neccessary to put them into practice.</t>
+  </si>
+  <si>
+    <t>These collection of General Hydrogen Fusion Plants provide plenty of options from personal portable units to plants that can power colony craft and can produce a respectable amount of power from any form of hydrogen. Indeed, you also have a number of options for open-chamber designs that can double as thrusters.</t>
+  </si>
+  <si>
+    <t>This collection of plasma weapons contain everythign from melee hold outs to orbital defence weapons. Though not the apex of this class of weapon, they do represent a collection of decent designs that could fill practically every need for an interstellar war-effort</t>
+  </si>
+  <si>
+    <t>From side-arms and concealable hold-outs to static emplacement and void-navy class weaponry, this series of laser weapons are decent examples of all scales of weaponry.</t>
+  </si>
+  <si>
+    <t>Splitting</t>
+  </si>
+  <si>
+    <t>Slicing</t>
+  </si>
+  <si>
+    <t>Piercing</t>
+  </si>
+  <si>
+    <t>Crushing</t>
+  </si>
+  <si>
+    <t>You know how to work your way into weaknesses, applying devasting force from within. You can create all sorts of tools to take advantage of this effect.</t>
+  </si>
+  <si>
+    <t>You know how to take advantage of the force you can produce over time concentrating and building up damage until you overcome your opponents defences. you know how to create all sorts of tools that take advantage of this effect.</t>
+  </si>
+  <si>
+    <t>You know how to build on overwhelming force, to destroy your foes though simply dealing more damage than they can handle. You know how to make tools of all sorts that enable you to vastly augment the forces you can bring to bear.</t>
+  </si>
+  <si>
+    <t>You know how to concetrate force, and even the strongest armour can only do so much if there is so little of it. You know how to take advantage of this effect to produce all sorts of tools.</t>
+  </si>
+  <si>
+    <t>You know how to create weapons intended for close-quarters combat. From daggers to spears, all forms of melee weaponry come easy to you and you can even design tools to best suit any user you care to name.</t>
+  </si>
+  <si>
+    <t>Strike True</t>
   </si>
 </sst>
 </file>
@@ -12819,8 +13035,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -13859,6 +14075,118 @@
         <v>1</v>
       </c>
     </row>
+    <row r="74" spans="1:4" ht="105" x14ac:dyDescent="0.35">
+      <c r="A74" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="C74" s="1">
+        <v>200</v>
+      </c>
+      <c r="D74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="147" x14ac:dyDescent="0.35">
+      <c r="A75" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="C75" s="1">
+        <v>200</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="168" x14ac:dyDescent="0.35">
+      <c r="A76" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C76" s="1">
+        <v>175</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A77" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="C77" s="1">
+        <v>200</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="63" x14ac:dyDescent="0.35">
+      <c r="A78" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="C78" s="1">
+        <v>25</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A79" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="C79" s="1">
+        <v>25</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="63" x14ac:dyDescent="0.35">
+      <c r="A80" s="7" t="s">
+        <v>783</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="C80" s="1">
+        <v>25</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A81" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="C81" s="1">
+        <v>25</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="12"/>
       <c r="B1048576" s="13"/>
@@ -13881,7 +14209,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -14303,6 +14631,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="30" spans="1:4" ht="63" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="C30" s="1">
+        <v>200</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048570" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048570" s="12"/>
       <c r="B1048570" s="13"/>
@@ -14324,8 +14666,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -14795,6 +15137,146 @@
         <v>1</v>
       </c>
     </row>
+    <row r="33" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A33" s="16" t="s">
+        <v>719</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="C33" s="4">
+        <v>150</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="147" x14ac:dyDescent="0.35">
+      <c r="A34" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="C34" s="4">
+        <v>150</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="126" x14ac:dyDescent="0.35">
+      <c r="A35" s="16" t="s">
+        <v>735</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="C35" s="4">
+        <v>100</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="126" x14ac:dyDescent="0.35">
+      <c r="A36" s="16" t="s">
+        <v>737</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="C36" s="4">
+        <v>100</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="105" x14ac:dyDescent="0.35">
+      <c r="A37" s="16" t="s">
+        <v>743</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="C37" s="4">
+        <v>750</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="63" x14ac:dyDescent="0.35">
+      <c r="A38" s="16" t="s">
+        <v>771</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="C38" s="4">
+        <v>150</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A39" s="16" t="s">
+        <v>772</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="C39" s="4">
+        <v>150</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="105" x14ac:dyDescent="0.35">
+      <c r="A40" s="16" t="s">
+        <v>773</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="C40" s="4">
+        <v>150</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.35">
+      <c r="A41" s="16" t="s">
+        <v>774</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="C41" s="4">
+        <v>150</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.35">
+      <c r="A42" s="16" t="s">
+        <v>775</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="C42" s="4">
+        <v>150</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="19"/>
       <c r="B1048576" s="14"/>
@@ -14815,9 +15297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1670431-A396-464E-A4B6-5555912D40B7}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="A29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -15270,6 +15752,40 @@
         <v>186</v>
       </c>
     </row>
+    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>754</v>
+      </c>
+      <c r="C27" s="4">
+        <v>350</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+      <c r="A28" s="16" t="s">
+        <v>755</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>756</v>
+      </c>
+      <c r="C28" s="4">
+        <v>350</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="19"/>
       <c r="B1048576" s="19"/>
@@ -15291,8 +15807,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -15693,6 +16209,23 @@
         <v>238</v>
       </c>
     </row>
+    <row r="24" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
+        <v>741</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C24" s="4">
+        <v>150</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>238</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="19"/>
       <c r="B1048576" s="13"/>
@@ -15713,9 +16246,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF76A29-35C0-4127-8FC4-384E3A5A7D3B}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -16110,6 +16643,48 @@
         <v>496</v>
       </c>
     </row>
+    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>746</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C27" s="1">
+        <v>200</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="12"/>
       <c r="B1048576" s="13"/>
@@ -16131,8 +16706,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -16469,6 +17044,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="22" spans="1:5" ht="126" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>751</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="C22" s="4">
+        <v>300</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="19"/>
       <c r="B1048576" s="13"/>
@@ -16490,8 +17079,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -16909,6 +17498,57 @@
         <v>237</v>
       </c>
     </row>
+    <row r="25" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
+        <v>749</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="C25" s="4">
+        <v>250</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
+        <v>767</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="C26" s="4">
+        <v>150</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>768</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="C27" s="4">
+        <v>300</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="19"/>
       <c r="B1048576" s="13"/>
@@ -16930,8 +17570,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -17328,6 +17968,23 @@
         <v>242</v>
       </c>
     </row>
+    <row r="25" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="C25" s="1">
+        <v>350</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="12"/>
       <c r="B1048576" s="13"/>
@@ -17349,8 +18006,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -17663,6 +18320,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="22" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="C22" s="1">
+        <v>300</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="C23" s="1">
+        <v>250</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="12"/>
       <c r="B1048576" s="13"/>
@@ -17684,8 +18369,8 @@
   <dimension ref="A1:E1048575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69:D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -18611,6 +19296,62 @@
         <v>200</v>
       </c>
       <c r="D65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="189" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="C66" s="1">
+        <v>200</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="63" x14ac:dyDescent="0.35">
+      <c r="A67" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="C67" s="1">
+        <v>200</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="126" x14ac:dyDescent="0.35">
+      <c r="A68" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C68" s="1">
+        <v>200</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="105" x14ac:dyDescent="0.35">
+      <c r="A69" s="16" t="s">
+        <v>757</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>758</v>
+      </c>
+      <c r="C69" s="4">
+        <v>200</v>
+      </c>
+      <c r="D69" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating version number and fixing perk classification
</commit_message>
<xml_diff>
--- a/perks.xlsx
+++ b/perks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fanfics\Tools\The March of Civilization Builder\March of Civilization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1C4EB1-D5FE-4318-A794-D9EEB2CF9A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D9D377-1E2F-460B-BE88-CC7E644A67CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{03648907-44A0-47E6-BAD5-79650EC445A4}"/>
+    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{03648907-44A0-47E6-BAD5-79650EC445A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="17" r:id="rId1"/>
@@ -2902,259 +2902,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -5456,6 +5203,199 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -5479,10 +5419,70 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -6417,42 +6417,42 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BCE785FF-FB68-4083-91B4-A2C662CAD8A3}" name="Basic" displayName="Basic" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BCE785FF-FB68-4083-91B4-A2C662CAD8A3}" name="Basic" displayName="Basic" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="A1:E1048576" xr:uid="{BCE785FF-FB68-4083-91B4-A2C662CAD8A3}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BEEAF5A3-CDBC-4D93-8920-D091DE98E8C2}" name="Name" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{A5C71F5A-5337-4825-9F2F-F44D681CE88A}" name="Description" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{1D31638B-1AF3-47F1-821C-DD8EF33F769E}" name="cost" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{697814DC-0D90-4F5B-86DE-7B42ADEBFCA5}" name="repeatable" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{12316AD0-2353-4186-B6DF-ED6D34E61FD8}" name="dependencies" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{BEEAF5A3-CDBC-4D93-8920-D091DE98E8C2}" name="Name" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{A5C71F5A-5337-4825-9F2F-F44D681CE88A}" name="Description" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{1D31638B-1AF3-47F1-821C-DD8EF33F769E}" name="cost" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{697814DC-0D90-4F5B-86DE-7B42ADEBFCA5}" name="repeatable" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{12316AD0-2353-4186-B6DF-ED6D34E61FD8}" name="dependencies" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97D8C2C7-5D85-45DA-94C8-1F9BE9DAEB58}" name="Powers" displayName="Powers" ref="A1:E1048570" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97D8C2C7-5D85-45DA-94C8-1F9BE9DAEB58}" name="Powers" displayName="Powers" ref="A1:E1048570" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:E1048570" xr:uid="{BCE785FF-FB68-4083-91B4-A2C662CAD8A3}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CB18EF03-1BFF-4D98-AB51-7EF51A818642}" name="Name" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{799187F2-EBB9-4754-B7ED-867F8B04BA18}" name="Description" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{E6E3ABD1-0FAE-496C-9DF0-F4C7B4902DE1}" name="cost" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{30246ED0-2FC9-4161-9DE7-ACA891847CF4}" name="repeatable" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{EA86C70B-2CF8-4DE3-86F5-CC0C41ED3875}" name="dependencies" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{CB18EF03-1BFF-4D98-AB51-7EF51A818642}" name="Name" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{799187F2-EBB9-4754-B7ED-867F8B04BA18}" name="Description" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E6E3ABD1-0FAE-496C-9DF0-F4C7B4902DE1}" name="cost" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{30246ED0-2FC9-4161-9DE7-ACA891847CF4}" name="repeatable" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{EA86C70B-2CF8-4DE3-86F5-CC0C41ED3875}" name="dependencies" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4FA86883-28A8-46A8-9D4D-7FE899360003}" name="Stuff" displayName="Stuff" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{4FA86883-28A8-46A8-9D4D-7FE899360003}" name="Stuff" displayName="Stuff" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E1048576" xr:uid="{BCE785FF-FB68-4083-91B4-A2C662CAD8A3}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{83277CAA-8B5E-44BB-9A68-8D7BDCBE7129}" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{0EA66C7E-7994-4EDB-8231-33D47336E877}" name="Description" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{71D9813A-93F1-457F-A812-49048CE52511}" name="cost" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{D2DFBD02-4993-4044-B35C-A6E9E6C86895}" name="repeatable" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{E660BDEE-8D44-4407-9AEC-FE291C2D3819}" name="dependencies" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{83277CAA-8B5E-44BB-9A68-8D7BDCBE7129}" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{0EA66C7E-7994-4EDB-8231-33D47336E877}" name="Description" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{71D9813A-93F1-457F-A812-49048CE52511}" name="cost" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D2DFBD02-4993-4044-B35C-A6E9E6C86895}" name="repeatable" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E660BDEE-8D44-4407-9AEC-FE291C2D3819}" name="dependencies" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6485,83 +6485,83 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{918E2B5F-AA90-4492-A772-D11F8CB2E76C}" name="Martial" displayName="Martial" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{918E2B5F-AA90-4492-A772-D11F8CB2E76C}" name="Martial" displayName="Martial" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86" totalsRowBorderDxfId="85">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{06F2E194-0AC3-4AA1-8CF3-6D6302A427F5}" name="Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C35CC3BC-6552-4937-B672-51786A17ACEF}" name="Description" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{61245F91-B3F3-4EC4-8F4F-6A9C570273D0}" name="cost" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{87442520-8C95-4470-9B68-9F920A6077A0}" name="repeatable" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{FEB08B9C-0382-4E01-878A-F3D013745B4C}" name="dependencies" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{06F2E194-0AC3-4AA1-8CF3-6D6302A427F5}" name="Name" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{C35CC3BC-6552-4937-B672-51786A17ACEF}" name="Description" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{61245F91-B3F3-4EC4-8F4F-6A9C570273D0}" name="cost" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{87442520-8C95-4470-9B68-9F920A6077A0}" name="repeatable" dataDxfId="81"/>
+    <tableColumn id="6" xr3:uid="{FEB08B9C-0382-4E01-878A-F3D013745B4C}" name="dependencies" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{87AB6AA4-70EE-4B7A-BCD2-54C42E9BF3D3}" name="Alchemy" displayName="Alchemy" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{87AB6AA4-70EE-4B7A-BCD2-54C42E9BF3D3}" name="Alchemy" displayName="Alchemy" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
   <autoFilter ref="A1:E1048576" xr:uid="{BCE785FF-FB68-4083-91B4-A2C662CAD8A3}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A8F452C0-4BA5-437D-A97D-3B852CFD3083}" name="Name" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{464DDAB9-9225-4607-8769-B112704486B7}" name="Description" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{5378E011-9C20-4E61-8110-19A742ADA4AF}" name="cost" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{85AD715E-C33F-44A5-951F-8F7E4EA85776}" name="repeatable" dataDxfId="78"/>
-    <tableColumn id="6" xr3:uid="{E60447CE-6283-459B-B687-2F7925CB9517}" name="dependencies" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{A8F452C0-4BA5-437D-A97D-3B852CFD3083}" name="Name" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{464DDAB9-9225-4607-8769-B112704486B7}" name="Description" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{5378E011-9C20-4E61-8110-19A742ADA4AF}" name="cost" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{85AD715E-C33F-44A5-951F-8F7E4EA85776}" name="repeatable" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{E60447CE-6283-459B-B687-2F7925CB9517}" name="dependencies" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5DC433FA-0132-48D5-890F-F980D0C30E30}" name="Magic" displayName="Magic" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75" tableBorderDxfId="73" totalsRowBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5DC433FA-0132-48D5-890F-F980D0C30E30}" name="Magic" displayName="Magic" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68" tableBorderDxfId="66" totalsRowBorderDxfId="65">
   <autoFilter ref="A1:E1048576" xr:uid="{5DC433FA-0132-48D5-890F-F980D0C30E30}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{312C94AC-C8AE-40C0-9931-2D45945BCCA5}" name="Name" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{E587CC06-2A33-444F-8CEB-BCA0056F8EE8}" name="Description" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{9E70A4DD-5296-4E79-8047-99A743951793}" name="cost" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{B5E8B616-0725-48D4-9D40-4771B8CB4CD3}" name="repeatable" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{80FC48F4-2EC1-43E3-9326-1D92420BC5BE}" name="dependencies" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{312C94AC-C8AE-40C0-9931-2D45945BCCA5}" name="Name" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{E587CC06-2A33-444F-8CEB-BCA0056F8EE8}" name="Description" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{9E70A4DD-5296-4E79-8047-99A743951793}" name="cost" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{B5E8B616-0725-48D4-9D40-4771B8CB4CD3}" name="repeatable" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{80FC48F4-2EC1-43E3-9326-1D92420BC5BE}" name="dependencies" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3FA3EDFE-B4D2-4319-942C-3099278BCB69}" name="Eldritch" displayName="Eldritch" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3FA3EDFE-B4D2-4319-942C-3099278BCB69}" name="Eldritch" displayName="Eldritch" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A1:E1048576" xr:uid="{3FA3EDFE-B4D2-4319-942C-3099278BCB69}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A8CF89CB-1F0A-4445-9934-A64D64AD1BD6}" name="Name" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{4580CFCD-3B94-4867-AF45-6548BED02616}" name="Description" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{4D13A38C-DA81-4630-BEDF-8094BF7E2F90}" name="cost" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{8D500541-70CA-4687-9A3B-0B260AE7A516}" name="repeatable" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{0841FEE4-6EF3-44AC-9EE8-495EA93D5C76}" name="dependencies" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{A8CF89CB-1F0A-4445-9934-A64D64AD1BD6}" name="Name" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{4580CFCD-3B94-4867-AF45-6548BED02616}" name="Description" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{4D13A38C-DA81-4630-BEDF-8094BF7E2F90}" name="cost" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{8D500541-70CA-4687-9A3B-0B260AE7A516}" name="repeatable" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{0841FEE4-6EF3-44AC-9EE8-495EA93D5C76}" name="dependencies" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6F16425C-6E87-4A26-AC81-3114C55ECE12}" name="Planar" displayName="Planar" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6F16425C-6E87-4A26-AC81-3114C55ECE12}" name="Planar" displayName="Planar" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="A1:E1048576" xr:uid="{6F16425C-6E87-4A26-AC81-3114C55ECE12}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A5FA7D5-7E79-4ACF-8E4D-C9EF1A0FC4B9}" name="Name" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{57D68A30-55BA-4874-A781-05B4A067F1F9}" name="Description" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{532F366A-5C01-44FC-88D3-2D756A155B94}" name="cost" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{570C2AC1-1F9C-4255-AABB-04A834F724D6}" name="repeatable" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{F1E75A1C-3975-464F-A10A-A78147F809E9}" name="dependencies" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{4A5FA7D5-7E79-4ACF-8E4D-C9EF1A0FC4B9}" name="Name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{57D68A30-55BA-4874-A781-05B4A067F1F9}" name="Description" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{532F366A-5C01-44FC-88D3-2D756A155B94}" name="cost" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{570C2AC1-1F9C-4255-AABB-04A834F724D6}" name="repeatable" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{F1E75A1C-3975-464F-A10A-A78147F809E9}" name="dependencies" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1FB923B5-8A9B-4B8B-B6FA-3C42807BB9B0}" name="Physics" displayName="Physics" ref="A1:E1048575" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="A1:E1048575" xr:uid="{1FB923B5-8A9B-4B8B-B6FA-3C42807BB9B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1FB923B5-8A9B-4B8B-B6FA-3C42807BB9B0}" name="Physics" displayName="Physics" ref="A1:E1048569" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+  <autoFilter ref="A1:E1048569" xr:uid="{1FB923B5-8A9B-4B8B-B6FA-3C42807BB9B0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BF975F14-62CF-49D8-8C3F-7B9FCB04C9C6}" name="Name" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{123D73EE-8504-46B4-9457-1B147F4D68AC}" name="Description" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{E042EE5D-4B0F-4AE1-AC39-418C7EE0DFB8}" name="cost" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{2E7646C6-4468-4049-B547-6562DC9AF21A}" name="repeatable" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{D8E2ED1A-34F5-4BE9-961F-CF685B0ABF9F}" name="dependencies" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{BF975F14-62CF-49D8-8C3F-7B9FCB04C9C6}" name="Name" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{123D73EE-8504-46B4-9457-1B147F4D68AC}" name="Description" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{E042EE5D-4B0F-4AE1-AC39-418C7EE0DFB8}" name="cost" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{2E7646C6-4468-4049-B547-6562DC9AF21A}" name="repeatable" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{D8E2ED1A-34F5-4BE9-961F-CF685B0ABF9F}" name="dependencies" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6866,8 +6866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888CE96D-9CC2-4BFE-ABB2-4D3AE4520CCE}">
   <dimension ref="A1:F352"/>
   <sheetViews>
-    <sheetView topLeftCell="A320" workbookViewId="0">
-      <selection activeCell="A327" sqref="A327"/>
+    <sheetView topLeftCell="B191" workbookViewId="0">
+      <selection activeCell="G197" sqref="G197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -14929,8 +14929,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -15568,6 +15568,90 @@
         <v>1</v>
       </c>
     </row>
+    <row r="45" spans="1:4" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C45" s="1">
+        <v>250</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C46" s="1">
+        <v>350</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="1" customFormat="1" ht="147" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C47" s="1">
+        <v>150</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C48" s="1">
+        <v>100</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="1" customFormat="1" ht="168" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C49" s="1">
+        <v>100</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C50" s="1">
+        <v>150</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1048576" s="19"/>
       <c r="B1048576" s="14"/>
@@ -15588,7 +15672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1670431-A396-464E-A4B6-5555912D40B7}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
@@ -18951,11 +19035,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8FCE86-AC21-49CB-A067-FEBC0A6D35BF}">
-  <dimension ref="A1:E1048575"/>
+  <dimension ref="A1:E1048569"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -19531,15 +19615,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="63" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>498</v>
+        <v>513</v>
       </c>
       <c r="C41" s="1">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -19547,27 +19631,27 @@
     </row>
     <row r="42" spans="1:4" ht="126" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>423</v>
+        <v>514</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>512</v>
+        <v>591</v>
       </c>
       <c r="C42" s="1">
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="105" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="126" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="C43" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -19575,13 +19659,13 @@
     </row>
     <row r="44" spans="1:4" ht="126" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>514</v>
+        <v>426</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C44" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -19589,10 +19673,10 @@
     </row>
     <row r="45" spans="1:4" ht="126" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C45" s="1">
         <v>250</v>
@@ -19603,10 +19687,10 @@
     </row>
     <row r="46" spans="1:4" ht="126" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C46" s="1">
         <v>250</v>
@@ -19615,54 +19699,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="126" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>427</v>
+        <v>453</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="C47" s="1">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="126" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="105" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
-        <v>428</v>
+        <v>520</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="C48" s="1">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="147" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="63" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
-        <v>429</v>
+        <v>641</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>517</v>
+        <v>645</v>
       </c>
       <c r="C49" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="E49" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
-        <v>443</v>
+        <v>642</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>594</v>
+        <v>646</v>
       </c>
       <c r="C50" s="1">
         <v>100</v>
@@ -19671,57 +19758,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="105" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>444</v>
+        <v>643</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>518</v>
+        <v>647</v>
       </c>
       <c r="C51" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="63" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
-        <v>453</v>
+        <v>644</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>519</v>
+        <v>648</v>
       </c>
       <c r="C52" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="168" x14ac:dyDescent="0.35">
-      <c r="A53" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="C53" s="1">
-        <v>100</v>
+    <row r="53" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+      <c r="A53" s="16" t="s">
+        <v>652</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="C53" s="4">
+        <v>300</v>
       </c>
       <c r="D53" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.35">
-      <c r="A54" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="C54" s="1">
-        <v>450</v>
+    <row r="54" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+      <c r="A54" s="16" t="s">
+        <v>653</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="C54" s="4">
+        <v>300</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
@@ -19729,10 +19816,10 @@
     </row>
     <row r="55" spans="1:5" ht="63" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
-        <v>641</v>
+        <v>662</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>645</v>
+        <v>663</v>
       </c>
       <c r="C55" s="1">
         <v>200</v>
@@ -19740,19 +19827,16 @@
       <c r="D55" s="1">
         <v>1</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="84" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
-        <v>642</v>
+        <v>677</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>646</v>
+        <v>709</v>
       </c>
       <c r="C56" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
@@ -19760,55 +19844,55 @@
     </row>
     <row r="57" spans="1:5" ht="105" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
-        <v>643</v>
+        <v>678</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>647</v>
+        <v>679</v>
       </c>
       <c r="C57" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="84" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
-        <v>644</v>
+        <v>684</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>648</v>
+        <v>710</v>
       </c>
       <c r="C58" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="63" x14ac:dyDescent="0.35">
-      <c r="A59" s="16" t="s">
-        <v>652</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>654</v>
-      </c>
-      <c r="C59" s="4">
-        <v>300</v>
+    <row r="59" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="C59" s="1">
+        <v>200</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="84" x14ac:dyDescent="0.35">
-      <c r="A60" s="16" t="s">
-        <v>653</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>655</v>
-      </c>
-      <c r="C60" s="4">
-        <v>300</v>
+    <row r="60" spans="1:5" ht="189" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="C60" s="1">
+        <v>200</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
@@ -19816,10 +19900,10 @@
     </row>
     <row r="61" spans="1:5" ht="63" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>662</v>
+        <v>723</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>663</v>
+        <v>724</v>
       </c>
       <c r="C61" s="1">
         <v>200</v>
@@ -19828,68 +19912,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="126" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
-        <v>677</v>
+        <v>739</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>709</v>
+        <v>740</v>
       </c>
       <c r="C62" s="1">
+        <v>200</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="A63" s="16" t="s">
+        <v>757</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>758</v>
+      </c>
+      <c r="C63" s="4">
+        <v>200</v>
+      </c>
+      <c r="D63" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="C64" s="1">
+        <v>200</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A65" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="C65" s="1">
         <v>150</v>
       </c>
-      <c r="D62" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="105" x14ac:dyDescent="0.35">
-      <c r="A63" s="7" t="s">
-        <v>678</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C63" s="1">
-        <v>200</v>
-      </c>
-      <c r="D63" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="84" x14ac:dyDescent="0.35">
-      <c r="A64" s="7" t="s">
-        <v>684</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="C64" s="1">
-        <v>200</v>
-      </c>
-      <c r="D64" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="105" x14ac:dyDescent="0.35">
-      <c r="A65" s="7" t="s">
-        <v>689</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>690</v>
-      </c>
-      <c r="C65" s="1">
-        <v>200</v>
-      </c>
       <c r="D65" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="189" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="84" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
-        <v>722</v>
+        <v>808</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>721</v>
+        <v>807</v>
       </c>
       <c r="C66" s="1">
         <v>200</v>
@@ -19898,110 +19982,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="63" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="84" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
-        <v>723</v>
+        <v>847</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>724</v>
+        <v>848</v>
       </c>
       <c r="C67" s="1">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="D67" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="126" x14ac:dyDescent="0.35">
-      <c r="A68" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="C68" s="1">
-        <v>200</v>
-      </c>
-      <c r="D68" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="105" x14ac:dyDescent="0.35">
-      <c r="A69" s="16" t="s">
-        <v>757</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>758</v>
-      </c>
-      <c r="C69" s="4">
-        <v>200</v>
-      </c>
-      <c r="D69" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="105" x14ac:dyDescent="0.35">
-      <c r="A70" s="7" t="s">
-        <v>795</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>796</v>
-      </c>
-      <c r="C70" s="1">
-        <v>200</v>
-      </c>
-      <c r="D70" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="84" x14ac:dyDescent="0.35">
-      <c r="A71" s="7" t="s">
-        <v>804</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>803</v>
-      </c>
-      <c r="C71" s="1">
-        <v>150</v>
-      </c>
-      <c r="D71" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="84" x14ac:dyDescent="0.35">
-      <c r="A72" s="7" t="s">
-        <v>808</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>807</v>
-      </c>
-      <c r="C72" s="1">
-        <v>200</v>
-      </c>
-      <c r="D72" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="84" x14ac:dyDescent="0.35">
-      <c r="A73" s="7" t="s">
-        <v>847</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>848</v>
-      </c>
-      <c r="C73" s="1">
-        <v>25</v>
-      </c>
-      <c r="D73" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1048575" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1048575" s="12"/>
-      <c r="B1048575" s="13"/>
-      <c r="C1048575" s="15"/>
-      <c r="D1048575" s="15"/>
-      <c r="E1048575" s="15"/>
+    <row r="1048569" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1048569" s="12"/>
+      <c r="B1048569" s="13"/>
+      <c r="C1048569" s="15"/>
+      <c r="D1048569" s="15"/>
+      <c r="E1048569" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>